<commit_message>
Añadido campo para tags en añadir pregunta
</commit_message>
<xml_diff>
--- a/docs/Bibliografía/División de los grupos.xlsx
+++ b/docs/Bibliografía/División de los grupos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\ICESI\Proyecto Integrador I\AssistMe\AssistMe-1\docs\Bibliografía\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDAB161-881D-498A-86F5-D7227AF2D019}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1280DD-25B2-40BC-8164-6C0349660503}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{E2089CE7-E6EE-4169-82E6-AD669CB74C35}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{E2089CE7-E6EE-4169-82E6-AD669CB74C35}"/>
   </bookViews>
   <sheets>
     <sheet name="Integrantes" sheetId="1" r:id="rId1"/>
@@ -208,7 +208,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -216,12 +216,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -232,6 +241,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -549,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA477D7C-ACEF-471D-BFF2-638301EA49BA}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07EDEE8E-7062-4E8F-9F68-D305F89C4771}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,117 +834,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>1.4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>2.7</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>3.1</v>
       </c>
-      <c r="F2">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2">
         <v>1.2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>1.5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>1.6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>3.2</v>
       </c>
-      <c r="F3">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
         <v>1.3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>1.7</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>2.1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>4.2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>3.3</v>
       </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>4.3</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>3.4</v>
       </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>3.5</v>
       </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2">
         <v>2.4</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>4.5</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>2.8</v>
       </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2">
         <v>2.5</v>
       </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2">
         <v>2.6</v>
       </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6">
         <v>2.7</v>
       </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>